<commit_message>
Fix bug do not show text with only placeholder in the cell
</commit_message>
<xml_diff>
--- a/test/templates/report.xlsx
+++ b/test/templates/report.xlsx
@@ -79,20 +79,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Địa chỉ: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>${Address}</t>
-    </r>
-  </si>
-  <si>
     <t>${table:TitleU}</t>
   </si>
   <si>
@@ -210,6 +196,9 @@
   </si>
   <si>
     <t>${table:TaskDetails}</t>
+  </si>
+  <si>
+    <t>${Address}</t>
   </si>
 </sst>
 </file>
@@ -347,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -390,6 +379,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -688,7 +678,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -713,30 +703,30 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
+      <c r="A2" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -744,7 +734,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="13"/>
@@ -759,7 +749,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="13"/>
@@ -774,7 +764,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="13"/>
@@ -789,7 +779,7 @@
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="13"/>
@@ -812,36 +802,36 @@
       <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" s="9" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19" t="s">
+      <c r="G10" s="20"/>
+      <c r="H10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="19"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:11" s="9" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
@@ -869,45 +859,45 @@
     </row>
     <row r="12" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="F12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="12">
         <f t="shared" ref="D13:K13" si="0">SUM(D12:D12)</f>
         <v>0</v>
@@ -949,11 +939,11 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="21" spans="5:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="11"/>

</xml_diff>